<commit_message>
Verified the tractor data and pushed the images again.
</commit_message>
<xml_diff>
--- a/Content/Tractor_images/digitrac.xlsx
+++ b/Content/Tractor_images/digitrac.xlsx
@@ -14,51 +14,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
-  <si>
-    <t>Trakstar Tractors</t>
-  </si>
-  <si>
-    <t>536</t>
-  </si>
-  <si>
-    <t>531</t>
-  </si>
-  <si>
-    <t>540</t>
-  </si>
-  <si>
-    <t>450</t>
-  </si>
-  <si>
-    <t>550</t>
-  </si>
-  <si>
-    <t>545 SMART</t>
-  </si>
-  <si>
-    <t>545</t>
-  </si>
-  <si>
-    <t>['img0-trakstar-536.png', 'img1-upload-1630737718-0.png', 'img2-upload-1630737718-0.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-trakstar-5316.png', 'img1-upload-1630738028-0.png', 'img2-upload-1630738028-0.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-trakstar-540.png', 'img1-upload-1630737836-0.png', 'img2-trakstar-540.png', 'img3-upload-1630737836-0.png']</t>
-  </si>
-  <si>
-    <t>['img0-450-1630737775.png', 'img1-upload-1630737775-0.png', 'img2-450-1630737775.png', 'img3-upload-1630737775-0.png']</t>
-  </si>
-  <si>
-    <t>['img0-trakstar-550.png', 'img1-upload-1630737889-0.png', 'img2-trakstar-550.png', 'img3-upload-1630737889-0.png']</t>
-  </si>
-  <si>
-    <t>['img0-trakstar-545-smart-1705646365.png', 'img1-trakstar-545-smart-17056463650.png', 'img2-trakstar-545-smart-1705646365.png', 'img3-trakstar-545-smart-17056463650.png']</t>
-  </si>
-  <si>
-    <t>['img0-trakstar-545.png', 'img1-upload-1642411587-0.png', 'img2-trakstar-545.png', 'img3-upload-1642411587-0.png']</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+  <si>
+    <t>Swaraj Tractors</t>
+  </si>
+  <si>
+    <t>855 FE</t>
+  </si>
+  <si>
+    <t>744 FE</t>
+  </si>
+  <si>
+    <t>735 FE</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>744 XT</t>
+  </si>
+  <si>
+    <t>742 XT</t>
+  </si>
+  <si>
+    <t>735 FE E</t>
+  </si>
+  <si>
+    <t>969 FE Trem IV-4wd</t>
+  </si>
+  <si>
+    <t>855 FE 4WD</t>
+  </si>
+  <si>
+    <t>744 FE 4WD</t>
+  </si>
+  <si>
+    <t>735 XT</t>
+  </si>
+  <si>
+    <t>['855FEimg0-swaraj-855-fe-1694259363.png', '855FEimg1-855-fe-1631015724.png', '855FEimg2-upload-1631015724-0.png']</t>
+  </si>
+  <si>
+    <t>['744FEimg0-swaraj-744-fe-1694259976.png', '744FEimg1-744-fe-1631014732.png', '744FEimg2-upload-1631014732-0.png']</t>
+  </si>
+  <si>
+    <t>['735FEimg0-735-fe-1631013770.png', '735FEimg1-mqdefault.png', '735FEimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['Codeimg0-code-1646204065.png', 'Codeimg1-code-1646204065.png', 'Codeimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['744XTimg0-swaraj-744-xt-1694260212.png', '744XTimg1-744-xt-1631015130.png', '744XTimg2-upload-1631015130-0.png']</t>
+  </si>
+  <si>
+    <t>['742XTimg0-swaraj-742-xt-1694259930.png', '742XTimg1-742-xt-1631014604.png', '742XTimg2-swaraj-742-xt-16942599300.png']</t>
+  </si>
+  <si>
+    <t>['735FEEimg0-swaraj-735-fe-e-1701335706.png', '735FEEimg1-swaraj-735-fe-e-17013357060.png', '735FEEimg2-swaraj-735-fe-e-1701335706.png']</t>
+  </si>
+  <si>
+    <t>['969FETremIV-4wdimg0-swaraj-969-fe-trem-iv-4wd-1689145707.png', '969FETremIV-4wdimg1-swaraj-969-fe-trem-iv-4wd-1689145707.png', '969FETremIV-4wdimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['855FE4WDimg0-swaraj-855-fe-4wd-1695808511.png', '855FE4WDimg1-swaraj-855-fe-4wd-16958103590.png', '855FE4WDimg2-swaraj-855-fe-4wd-16958103590.png']</t>
+  </si>
+  <si>
+    <t>['744FE4WDimg0-744-fe-4wd-1631014809.png', '744FE4WDimg1-mqdefault.png', '744FE4WDimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['735XTimg0-735-xt-1631014365.png', '735XTimg1-735-xt-1631014365.png', '735XTimg2-mqdefault.png']</t>
   </si>
   <si>
     <t>Brand</t>
@@ -423,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -431,13 +455,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -448,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -459,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -470,7 +494,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -481,7 +505,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -492,7 +516,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -503,7 +527,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -514,7 +538,51 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scraped the left tractor images.
</commit_message>
<xml_diff>
--- a/Content/Tractor_images/digitrac.xlsx
+++ b/Content/Tractor_images/digitrac.xlsx
@@ -14,75 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
-  <si>
-    <t>Swaraj Tractors</t>
-  </si>
-  <si>
-    <t>855 FE</t>
-  </si>
-  <si>
-    <t>744 FE</t>
-  </si>
-  <si>
-    <t>735 FE</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>744 XT</t>
-  </si>
-  <si>
-    <t>742 XT</t>
-  </si>
-  <si>
-    <t>735 FE E</t>
-  </si>
-  <si>
-    <t>969 FE Trem IV-4wd</t>
-  </si>
-  <si>
-    <t>855 FE 4WD</t>
-  </si>
-  <si>
-    <t>744 FE 4WD</t>
-  </si>
-  <si>
-    <t>735 XT</t>
-  </si>
-  <si>
-    <t>['855FEimg0-swaraj-855-fe-1694259363.png', '855FEimg1-855-fe-1631015724.png', '855FEimg2-upload-1631015724-0.png']</t>
-  </si>
-  <si>
-    <t>['744FEimg0-swaraj-744-fe-1694259976.png', '744FEimg1-744-fe-1631014732.png', '744FEimg2-upload-1631014732-0.png']</t>
-  </si>
-  <si>
-    <t>['735FEimg0-735-fe-1631013770.png', '735FEimg1-mqdefault.png', '735FEimg2-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['Codeimg0-code-1646204065.png', 'Codeimg1-code-1646204065.png', 'Codeimg2-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['744XTimg0-swaraj-744-xt-1694260212.png', '744XTimg1-744-xt-1631015130.png', '744XTimg2-upload-1631015130-0.png']</t>
-  </si>
-  <si>
-    <t>['742XTimg0-swaraj-742-xt-1694259930.png', '742XTimg1-742-xt-1631014604.png', '742XTimg2-swaraj-742-xt-16942599300.png']</t>
-  </si>
-  <si>
-    <t>['735FEEimg0-swaraj-735-fe-e-1701335706.png', '735FEEimg1-swaraj-735-fe-e-17013357060.png', '735FEEimg2-swaraj-735-fe-e-1701335706.png']</t>
-  </si>
-  <si>
-    <t>['969FETremIV-4wdimg0-swaraj-969-fe-trem-iv-4wd-1689145707.png', '969FETremIV-4wdimg1-swaraj-969-fe-trem-iv-4wd-1689145707.png', '969FETremIV-4wdimg2-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['855FE4WDimg0-swaraj-855-fe-4wd-1695808511.png', '855FE4WDimg1-swaraj-855-fe-4wd-16958103590.png', '855FE4WDimg2-swaraj-855-fe-4wd-16958103590.png']</t>
-  </si>
-  <si>
-    <t>['744FE4WDimg0-744-fe-4wd-1631014809.png', '744FE4WDimg1-mqdefault.png', '744FE4WDimg2-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['735XTimg0-735-xt-1631014365.png', '735XTimg1-735-xt-1631014365.png', '735XTimg2-mqdefault.png']</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+  <si>
+    <t>Sonalika Tractors</t>
+  </si>
+  <si>
+    <t>DI 35</t>
+  </si>
+  <si>
+    <t>745 DI III Sikander</t>
+  </si>
+  <si>
+    <t>Tiger 50</t>
+  </si>
+  <si>
+    <t>DI 750III</t>
+  </si>
+  <si>
+    <t>Tiger Electric 4WD</t>
+  </si>
+  <si>
+    <t>DI 60</t>
+  </si>
+  <si>
+    <t>DI 42 RX</t>
+  </si>
+  <si>
+    <t>DI 745 III</t>
+  </si>
+  <si>
+    <t>42 DI Sikander</t>
+  </si>
+  <si>
+    <t>WT 60</t>
+  </si>
+  <si>
+    <t>['DI35img0-di-35-1631526570.png', 'DI35img1-mqdefault.png', 'DI35img2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['745DIIIISikanderimg0-745-di-iii-sikander-1631526194.png', '745DIIIISikanderimg1-upload-1631526194-0.png', '745DIIIISikanderimg2-upload-1631526194-0.png']</t>
+  </si>
+  <si>
+    <t>['Tiger50img0-tiger-50-1631530291.png', 'Tiger50img1-upload-1631530291-0.png', 'Tiger50img2-upload-1631530291-0.png']</t>
+  </si>
+  <si>
+    <t>['DI750IIIimg0-di-750iii-1631529270.png', 'DI750IIIimg1-upload-1631529270-0.png', 'DI750IIIimg2-di-750iii-1631529270.png']</t>
+  </si>
+  <si>
+    <t>['TigerElectric4WDimg0-sonalika-tiger-electric-4wd-1696505405.png', 'TigerElectric4WDimg1-sonalika-tiger-electric-4wd-16965054050.png', 'TigerElectric4WDimg2-sonalika-tiger-electric-4wd-1696505405.png']</t>
+  </si>
+  <si>
+    <t>['DI60img0-di-60-1631527166.png', 'DI60img1-upload-1631527166-0.png', 'DI60img2-upload-1631527166-0.png']</t>
+  </si>
+  <si>
+    <t>['DI42RXimg0-di-42-rx-1631526666.png', 'DI42RXimg1-di-42-rx-1631526666.png', 'DI42RXimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['DI745IIIimg0-di-745-iii-1631528823.png', 'DI745IIIimg1-upload-1631528823-0.png', 'DI745IIIimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['42DISikanderimg0-42-di-sikander-1631525877.png', '42DISikanderimg1-upload-1631525877-0.png', '42DISikanderimg2-upload-1631525877-0.png']</t>
+  </si>
+  <si>
+    <t>['WT60img0-wt-60-1631530732.png', 'WT60img1-upload-1631530732-0.png', 'WT60img2-wt-60-1631530732.png']</t>
   </si>
   <si>
     <t>Brand</t>
@@ -455,13 +449,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -472,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -483,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -491,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -502,10 +496,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -513,10 +507,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -524,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -535,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -546,10 +540,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -557,10 +551,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -568,10 +562,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -579,10 +573,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>